<commit_message>
reorganise le projet avec une couche services. CurveService generera les axes et les datasets
</commit_message>
<xml_diff>
--- a/featuresTodo.xlsx
+++ b/featuresTodo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxime Pageot\Documents\PapaPlotProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EFB129-A8F8-47D8-872D-5B3D1C4F11C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74DB46B-4576-4539-9CF2-FBE9A969D4BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BA8DB4F9-20D0-4A37-956E-904E12834BB3}"/>
   </bookViews>
@@ -36,15 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Add Track</t>
   </si>
   <si>
     <t>Add Curve</t>
-  </si>
-  <si>
-    <t>MVP</t>
   </si>
   <si>
     <t>Editing Curve</t>
@@ -473,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD5EB67-553C-4C24-ACB4-00A1615F019D}">
-  <dimension ref="A1:A22"/>
+  <dimension ref="A2:A22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,11 +482,6 @@
     <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
@@ -502,97 +494,97 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>